<commit_message>
after tasks page testcase
</commit_message>
<xml_diff>
--- a/src/main/resources/CRMTestData.xlsx
+++ b/src/main/resources/CRMTestData.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\learning j\SeleniumFrameWork\SeleniumFrameWork\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2472" windowWidth="12012" windowHeight="4308" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2475" windowWidth="12015" windowHeight="4305" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
     <sheet name="Deals" sheetId="4" r:id="rId2"/>
     <sheet name="Tasks" sheetId="5" r:id="rId3"/>
+    <sheet name="Search_Name" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Title</t>
   </si>
@@ -65,12 +71,21 @@
   <si>
     <t>Sharma</t>
   </si>
+  <si>
+    <t>Sl No</t>
+  </si>
+  <si>
+    <t>Detail</t>
+  </si>
+  <si>
+    <t>search by details</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -128,12 +143,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -180,7 +205,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,9 +237,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,6 +272,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -421,22 +448,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -450,7 +476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -464,7 +490,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -478,7 +504,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
@@ -498,25 +524,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
after my new frame work addition
</commit_message>
<xml_diff>
--- a/src/main/resources/CRMTestData.xlsx
+++ b/src/main/resources/CRMTestData.xlsx
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2475" windowWidth="12015" windowHeight="4305" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="2475" windowWidth="12015" windowHeight="4305" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="Deals" sheetId="4" r:id="rId2"/>
-    <sheet name="Tasks" sheetId="5" r:id="rId3"/>
-    <sheet name="Search_Name" sheetId="6" r:id="rId4"/>
+    <sheet name="Tasks" sheetId="5" r:id="rId2"/>
+    <sheet name="DealsPageFullSearchPage" sheetId="6" r:id="rId3"/>
+    <sheet name="DealsPageDate" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Title</t>
   </si>
@@ -72,21 +72,86 @@
     <t>Sharma</t>
   </si>
   <si>
-    <t>Sl No</t>
-  </si>
-  <si>
-    <t>Detail</t>
-  </si>
-  <si>
-    <t>search by details</t>
+    <t>New</t>
+  </si>
+  <si>
+    <t>AMEER SALMAN</t>
+  </si>
+  <si>
+    <t>Existing Customer</t>
+  </si>
+  <si>
+    <t>Equal to</t>
+  </si>
+  <si>
+    <t>CreationFrom</t>
+  </si>
+  <si>
+    <t>CreationTo</t>
+  </si>
+  <si>
+    <t>ModifiedFrom</t>
+  </si>
+  <si>
+    <t>ModifiedTo</t>
+  </si>
+  <si>
+    <t>CloseDate</t>
+  </si>
+  <si>
+    <t>Data Types</t>
+  </si>
+  <si>
+    <t>Data1</t>
+  </si>
+  <si>
+    <t>Data2</t>
+  </si>
+  <si>
+    <t>Data3</t>
+  </si>
+  <si>
+    <t>Data4</t>
+  </si>
+  <si>
+    <t>Data5</t>
+  </si>
+  <si>
+    <t>DatesForDealsPage</t>
+  </si>
+  <si>
+    <t>dropDownValues</t>
+  </si>
+  <si>
+    <t>12/04/2022</t>
+  </si>
+  <si>
+    <t>12/07/2022</t>
+  </si>
+  <si>
+    <t>05/10/2022</t>
+  </si>
+  <si>
+    <t>10/10/2022</t>
+  </si>
+  <si>
+    <t>12/12/2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -135,7 +200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -144,7 +209,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,43 +612,133 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" activeCellId="1" sqref="A2 A2:A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>44663</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44754</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44839</v>
+      </c>
+      <c r="D2" s="4">
+        <v>44844</v>
+      </c>
+      <c r="E2" s="4">
+        <v>44907</v>
       </c>
     </row>
   </sheetData>

</xml_diff>